<commit_message>
Excels unificados. Modificacion a [universidad.py] para que lo implemente
Se combinaron los archivos anteriores de Edificios y Aulas, en el excel 'Universidad.xlsx', borrando luego los archivos redundantes.
Modificacion a [universidad.py] para que correctamente importe los dataframes a partir de los sheets del excel. El cambio realiza la accion correctamente y no rompe el funcionamiento existente a la hora de realizar este push.
</commit_message>
<xml_diff>
--- a/src/assets/edificios_default/Universidad.xlsx
+++ b/src/assets/edificios_default/Universidad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Edificios" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
   <si>
     <t xml:space="preserve">Edificio</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacidad</t>
   </si>
   <si>
     <t xml:space="preserve">Equipamiento</t>
@@ -175,7 +178,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,10 +189,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -341,10 +340,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -353,53 +352,59 @@
       <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="0" t="s">
-        <v>18</v>
+      <c r="K1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>19</v>
-      </c>
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>20</v>
-      </c>
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>21</v>
-      </c>
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Debe usar un edificio ya instanciado para esta celda" promptTitle="Error_Edificio" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B2:B1004" type="custom">
-      <formula1>#¿NOMBRE?</formula1>
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" prompt="Debe usar un edificio ya instanciado para esta celda" promptTitle="Error_Edificio" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C1004" type="custom">
+      <formula1>#¿nombre?</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -426,15 +431,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -455,7 +460,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Agregado de tablas de backend para empezar pruebas
- Añadi dos hojas, 'aulas_compatibles_backend' y 'materias_compatibles_backend' al excel que se instancia inicialmente en la universidad. Sus dataframes correspondientes se generan al instanciar el objeto Universidad, como atributos del mismo.
- Agregado de los dataframes faltantes a Universidad.py, faltan metodos para interactuar con UI con los dataframes nuevos
</commit_message>
<xml_diff>
--- a/src/assets/edificios_default/Universidad.xlsx
+++ b/src/assets/edificios_default/Universidad.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Edificios" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Aulas" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Carreras" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Materias" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="aulas_compatibles_backend" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="clases_compatibles_backend" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="87">
   <si>
     <t xml:space="preserve">Edificio</t>
   </si>
@@ -85,19 +87,205 @@
     <t xml:space="preserve">Equipamiento</t>
   </si>
   <si>
-    <t xml:space="preserve">B-101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B-102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B-103</t>
+    <t xml:space="preserve">B102-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7:00-23:00 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">proyector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B102-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proyector, híbrido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B202-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B202-A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proyector, computadoras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pecera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B202</t>
   </si>
   <si>
     <t xml:space="preserve">Carrera</t>
   </si>
   <si>
     <t xml:space="preserve">Preferencia de Edificio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingeniería en Computación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingeniería Electrónica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingeniería Ambiental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenciatura en Economía</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Código</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Año</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edificio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equipamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_lunes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_martes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_miércoles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_jueves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_viernes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_sábado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">día</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horario_inicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horario_fin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cantidad_de_alumnos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equipamiento_necesario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edificio_preferido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I - Teórica C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jueves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I- Práctica C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">miércoles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I - Teórica C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">martes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I- Práctica C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lunes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I - Teórica C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I- Práctica C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">viernes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6001 - Introducción a la Ing. En Computación - C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T0002 - ILEA - C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T0002 - ILEA - C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6006 - Matematica II - Teórica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6006 - Matematica II - Práctica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6008 - Programación II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">computadoras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6009 - Arquitectura de Computadoras I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6011 - Física General II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6013 - Bases de Datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6016 - Laboratorio de Sistemas Embebidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6017 - Seguridad Ambiental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6022 - PEPA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B5672 - Comunicaciones Analógicas y Digitales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6038 - Economía y Organización Industrial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sábado</t>
   </si>
 </sst>
 </file>
@@ -178,7 +366,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -189,10 +377,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -215,7 +399,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -344,10 +528,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -388,35 +572,355 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="0" t="n">
+        <v>40</v>
+      </c>
       <c r="C2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="0" t="n">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="0" t="s">
-        <v>14</v>
+      <c r="C9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" prompt="Debe usar un edificio ya instanciado para esta celda" promptTitle="Error_Edificio" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C2:C1004" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" prompt="Debe usar un edificio ya instanciado para esta celda" promptTitle="Error_Edificio" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C12:C1001" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -436,23 +940,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -471,14 +1002,960 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.25"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.36"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Generacion de nombres concatenados, para dropdownear en config_horarios
</commit_message>
<xml_diff>
--- a/src/assets/edificios_default/Universidad.xlsx
+++ b/src/assets/edificios_default/Universidad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Edificios" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="102">
   <si>
     <t xml:space="preserve">Edificio</t>
   </si>
@@ -154,6 +154,9 @@
     <t xml:space="preserve">Nombre</t>
   </si>
   <si>
+    <t xml:space="preserve">Comision</t>
+  </si>
+  <si>
     <t xml:space="preserve">Año</t>
   </si>
   <si>
@@ -181,6 +184,30 @@
     <t xml:space="preserve">Miercoles</t>
   </si>
   <si>
+    <t xml:space="preserve">Día</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horario de inicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horario de fin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cantidad de alumnos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipamiento necesario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edificio preferencial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aula_asignada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mate I comision 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">edificio</t>
   </si>
   <si>
@@ -224,9 +251,6 @@
   </si>
   <si>
     <t xml:space="preserve">edificio_preferido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aula_asignada</t>
   </si>
   <si>
     <t xml:space="preserve">B6000 - Matematica I - Teórica C1</t>
@@ -965,7 +989,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1024,17 +1048,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1045,53 +1070,56 @@
         <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>46</v>
+      <c r="A2" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="1" t="n">
+      <c r="E3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>50</v>
+      <c r="F3" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1110,14 +1138,58 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1136,7 +1208,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1152,34 +1224,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,22 +1268,22 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1228,22 +1300,22 @@
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1260,22 +1332,22 @@
         <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1292,22 +1364,22 @@
         <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,22 +1396,22 @@
         <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,22 +1428,22 @@
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,22 +1460,22 @@
         <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1417,19 +1489,19 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1446,22 +1518,22 @@
         <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1478,22 +1550,22 @@
         <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1514,8 +1586,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1526,41 +1598,41 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>11</v>
@@ -1580,10 +1652,10 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>15</v>
@@ -1600,10 +1672,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>13</v>
@@ -1623,10 +1695,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>15</v>
@@ -1643,10 +1715,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>17</v>
@@ -1666,10 +1738,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>9</v>
@@ -1686,10 +1758,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>17</v>
@@ -1706,10 +1778,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>15</v>
@@ -1723,10 +1795,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>15</v>
@@ -1740,10 +1812,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>19</v>
@@ -1757,10 +1829,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>19</v>
@@ -1774,10 +1846,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>11</v>
@@ -1797,10 +1869,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>11</v>
@@ -1817,10 +1889,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>17</v>
@@ -1840,10 +1912,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>18</v>
@@ -1855,7 +1927,7 @@
         <v>75</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>14</v>
@@ -1863,10 +1935,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>20</v>
@@ -1886,10 +1958,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>9</v>
@@ -1906,10 +1978,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>18</v>
@@ -1929,10 +2001,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>17</v>
@@ -1949,10 +2021,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>13</v>
@@ -1966,10 +2038,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>19</v>
@@ -1989,10 +2061,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>13</v>
@@ -2012,10 +2084,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>13</v>
@@ -2032,10 +2104,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>8</v>

</xml_diff>

<commit_message>
Cambios a Universidad.xlsx para incluir casos de prueba previos
</commit_message>
<xml_diff>
--- a/src/assets/edificios_default/Universidad.xlsx
+++ b/src/assets/edificios_default/Universidad.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="118">
   <si>
     <t xml:space="preserve">Edificio</t>
   </si>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">Nombre</t>
   </si>
   <si>
-    <t xml:space="preserve">Comision</t>
+    <t xml:space="preserve">Comisión</t>
   </si>
   <si>
     <t xml:space="preserve">Año</t>
@@ -175,12 +175,18 @@
     <t xml:space="preserve">Matematica I</t>
   </si>
   <si>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
     <t xml:space="preserve">ICOMP</t>
   </si>
   <si>
     <t xml:space="preserve">B60002</t>
   </si>
   <si>
+    <t xml:space="preserve">C2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Miercoles</t>
   </si>
   <si>
@@ -202,133 +208,383 @@
     <t xml:space="preserve">Edificio preferencial</t>
   </si>
   <si>
+    <t xml:space="preserve">Aula asignada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I - Teórica C1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B6006 - Matematica II - Práctica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B5672 - Comunicaciones Analógicas y Digitales</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">13</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I - Teórica C3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">17</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B6001 - Introducción a la Ing. En Computación - C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I- Práctica C2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B6006 - Matematica II - Teórica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I - Teórica C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T0002 - ILEA - C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I- Práctica C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6008 - Programación II</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">20</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">T0002 - ILEA – C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6009 - Arquitectura de Computadoras I</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">23</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B6038 - Economía y Organización Industrial</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">12</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B6017 - Seguridad Ambiental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6016 - Laboratorio de Sistemas Embebidos</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">computadoras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T0002 - ILEA - C2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6000 - Matematica I- Práctica C3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">:00</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">B6011 - Física General II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edificio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equipamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_lunes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_martes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_miércoles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_jueves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_viernes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">horarios_sábado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7,23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">día</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cantidad_de_alumnos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">equipamiento_necesario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edificio_preferido</t>
+  </si>
+  <si>
     <t xml:space="preserve">aula_asignada</t>
   </si>
   <si>
-    <t xml:space="preserve">Mate I comision 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edificio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capacidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">equipamiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_lunes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_martes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_miércoles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_jueves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_viernes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_sábado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">día</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cantidad_de_alumnos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">equipamiento_necesario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edificio_preferido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6000 - Matematica I - Teórica C1</t>
-  </si>
-  <si>
     <t xml:space="preserve">jueves</t>
   </si>
   <si>
-    <t xml:space="preserve">B6000 - Matematica I- Práctica C1</t>
-  </si>
-  <si>
     <t xml:space="preserve">miércoles</t>
   </si>
   <si>
-    <t xml:space="preserve">B6000 - Matematica I - Teórica C2</t>
-  </si>
-  <si>
     <t xml:space="preserve">martes</t>
   </si>
   <si>
-    <t xml:space="preserve">B6000 - Matematica I- Práctica C2</t>
-  </si>
-  <si>
     <t xml:space="preserve">lunes</t>
   </si>
   <si>
-    <t xml:space="preserve">B6000 - Matematica I - Teórica C3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6000 - Matematica I- Práctica C3</t>
-  </si>
-  <si>
     <t xml:space="preserve">viernes</t>
   </si>
   <si>
-    <t xml:space="preserve">B6001 - Introducción a la Ing. En Computación - C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T0002 - ILEA - C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T0002 - ILEA - C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6006 - Matematica II - Teórica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6006 - Matematica II - Práctica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6008 - Programación II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">computadoras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6009 - Arquitectura de Computadoras I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6011 - Física General II</t>
-  </si>
-  <si>
     <t xml:space="preserve">B6013 - Bases de Datos</t>
   </si>
   <si>
-    <t xml:space="preserve">B6016 - Laboratorio de Sistemas Embebidos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6017 - Seguridad Ambiental</t>
-  </si>
-  <si>
     <t xml:space="preserve">B6022 - PEPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B5672 - Comunicaciones Analógicas y Digitales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6038 - Economía y Organización Industrial</t>
   </si>
   <si>
     <t xml:space="preserve">sábado</t>
@@ -338,10 +594,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -368,6 +625,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -412,7 +674,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -425,6 +687,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,6 +700,15 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -577,7 +852,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -966,7 +1241,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" prompt="Debe usar un edificio ya instanciado para esta celda" promptTitle="Error_Edificio" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C12:C1001" type="none">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" prompt="Debe usar un edificio ya instanciado para esta celda" promptTitle="Error_Edificio" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="C12:C999" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1051,7 +1326,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1095,8 +1370,11 @@
       <c r="B2" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -1107,19 +1385,22 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="D3" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1138,15 +1419,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.05"/>
@@ -1160,34 +1441,554 @@
         <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>59</v>
-      </c>
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1208,7 +2009,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1224,34 +2025,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1268,22 +2069,22 @@
         <v>22</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,22 +2101,22 @@
         <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,22 +2133,22 @@
         <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,22 +2165,22 @@
         <v>22</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,22 +2197,22 @@
         <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1428,22 +2229,22 @@
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1460,22 +2261,22 @@
         <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1489,19 +2290,19 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,22 +2319,22 @@
         <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,22 +2351,22 @@
         <v>22</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1586,8 +2387,8 @@
   </sheetPr>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1603,10 +2404,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>45</v>
@@ -1615,24 +2416,24 @@
         <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>58</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>11</v>
@@ -1655,7 +2456,7 @@
         <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>15</v>
@@ -1672,10 +2473,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>13</v>
@@ -1695,10 +2496,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>15</v>
@@ -1715,10 +2516,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>17</v>
@@ -1738,10 +2539,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>9</v>
@@ -1758,10 +2559,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>17</v>
@@ -1778,10 +2579,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>15</v>
@@ -1795,10 +2596,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>15</v>
@@ -1812,10 +2613,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>19</v>
@@ -1829,10 +2630,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>19</v>
@@ -1846,10 +2647,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>11</v>
@@ -1869,10 +2670,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>11</v>
@@ -1889,10 +2690,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>17</v>
@@ -1912,10 +2713,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>18</v>
@@ -1927,7 +2728,7 @@
         <v>75</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>14</v>
@@ -1935,10 +2736,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>20</v>
@@ -1958,10 +2759,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>9</v>
@@ -1978,10 +2779,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>18</v>
@@ -2001,10 +2802,10 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>17</v>
@@ -2021,10 +2822,10 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>13</v>
@@ -2038,10 +2839,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>19</v>
@@ -2061,10 +2862,10 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>13</v>
@@ -2084,10 +2885,10 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>13</v>
@@ -2104,10 +2905,10 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>8</v>

</xml_diff>

<commit_message>
Conexion con backend hardcodeada por ahora, funciona
</commit_message>
<xml_diff>
--- a/src/assets/edificios_default/Universidad.xlsx
+++ b/src/assets/edificios_default/Universidad.xlsx
@@ -13,8 +13,6 @@
     <sheet name="Carreras" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Materias" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Clases" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="aulas_compatibles_backend" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="clases_compatibles_backend" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="94">
   <si>
     <t xml:space="preserve">Edificio</t>
   </si>
@@ -516,78 +514,6 @@
   </si>
   <si>
     <t xml:space="preserve">B6011 - Física General II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edificio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nombre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capacidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">equipamiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_lunes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_martes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_miércoles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_jueves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_viernes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horarios_sábado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7,23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">día</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cantidad_de_alumnos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">equipamiento_necesario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edificio_preferido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aula_asignada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jueves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">miércoles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">martes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lunes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">viernes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6013 - Bases de Datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B6022 - PEPA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sábado</t>
   </si>
 </sst>
 </file>
@@ -1421,8 +1347,8 @@
   </sheetPr>
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1433,7 +1359,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1458,11 +1385,11 @@
       <c r="G1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,7 +1414,7 @@
       <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="H2" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1511,7 +1438,7 @@
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="H3" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1535,7 +1462,7 @@
       <c r="G4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="H4" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1561,7 +1488,7 @@
       <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="H5" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1585,7 +1512,7 @@
       <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="H6" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1609,7 +1536,7 @@
       <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="H7" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1635,7 +1562,7 @@
       <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1661,7 +1588,7 @@
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="H9" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1685,7 +1612,7 @@
       <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="H10" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1709,7 +1636,7 @@
       <c r="G11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="H11" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1735,7 +1662,7 @@
       <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1759,7 +1686,7 @@
       <c r="G13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1785,7 +1712,7 @@
       <c r="G14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="H14" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1809,7 +1736,7 @@
       <c r="G15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="H15" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1833,7 +1760,7 @@
       <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="H16" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1857,7 +1784,7 @@
       <c r="G17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="H17" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1881,7 +1808,7 @@
       <c r="G18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="H18" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1907,7 +1834,7 @@
       <c r="G19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="H19" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1931,7 +1858,7 @@
       <c r="G20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="H20" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1955,7 +1882,7 @@
       <c r="G21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="H21" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1979,7 +1906,7 @@
       <c r="G22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="H22" s="0" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1989,936 +1916,6 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:J11"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="20.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.51"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H25"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="44.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="21.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.55"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C9" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C10" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>80</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C22" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="E22" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C23" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="E23" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C24" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="E24" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C25" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="D25" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="E25" s="1" t="n">
-        <v>30</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
limpieza de metodo de asignacion
</commit_message>
<xml_diff>
--- a/src/assets/edificios_default/Universidad.xlsx
+++ b/src/assets/edificios_default/Universidad.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="111">
   <si>
     <t xml:space="preserve">Edificio</t>
   </si>
@@ -158,34 +158,85 @@
     <t xml:space="preserve">Año</t>
   </si>
   <si>
-    <t xml:space="preserve">Dia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horario_inicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">horario_fin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B60001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matematica I</t>
+    <t xml:space="preserve">B6000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matematica I - Teórica</t>
   </si>
   <si>
     <t xml:space="preserve">C1</t>
   </si>
   <si>
-    <t xml:space="preserve">ICOMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B60002</t>
+    <t xml:space="preserve">B6006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matematica II - Práctica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B5672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comunicaciones Analógicas y Digitales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introducción a la Ing. En Computación</t>
   </si>
   <si>
     <t xml:space="preserve">C2</t>
   </si>
   <si>
-    <t xml:space="preserve">Miercoles</t>
+    <t xml:space="preserve">Matematica I - Práctica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matematica II - Teórica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILEA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Programación II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arquitectura de Computadoras I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6038</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Economía y Organización Industrial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seguridad Ambiental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laboratorio de Sistemas Embebidos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B6011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Física General II</t>
   </si>
   <si>
     <t xml:space="preserve">Día</t>
@@ -200,54 +251,22 @@
     <t xml:space="preserve">Cantidad de alumnos</t>
   </si>
   <si>
+    <t xml:space="preserve">Aula asignada</t>
+  </si>
+  <si>
     <t xml:space="preserve">Equipamiento necesario</t>
   </si>
   <si>
     <t xml:space="preserve">Edificio preferencial</t>
   </si>
   <si>
-    <t xml:space="preserve">Aula asignada</t>
-  </si>
-  <si>
     <t xml:space="preserve">B6000 - Matematica I - Teórica C1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">11</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
+    <t xml:space="preserve">11:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15:00</t>
   </si>
   <si>
     <t xml:space="preserve">B6006 - Matematica II - Práctica</t>
@@ -256,83 +275,19 @@
     <t xml:space="preserve">B5672 - Comunicaciones Analógicas y Digitales</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">13</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">16</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
+    <t xml:space="preserve">13:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16:00</t>
   </si>
   <si>
     <t xml:space="preserve">B6000 - Matematica I - Teórica C3</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">17</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">21</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
+    <t xml:space="preserve">17:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21:00</t>
   </si>
   <si>
     <t xml:space="preserve">B6001 - Introducción a la Ing. En Computación - C2</t>
@@ -341,23 +296,7 @@
     <t xml:space="preserve">B6000 - Matematica I- Práctica C2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">19</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
+    <t xml:space="preserve">19:00</t>
   </si>
   <si>
     <t xml:space="preserve">B6006 - Matematica II - Teórica</t>
@@ -375,23 +314,7 @@
     <t xml:space="preserve">B6008 - Programación II</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">20</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
+    <t xml:space="preserve">20:00</t>
   </si>
   <si>
     <t xml:space="preserve">T0002 - ILEA – C2</t>
@@ -400,64 +323,16 @@
     <t xml:space="preserve">B6009 - Arquitectura de Computadoras I</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">23</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
+    <t xml:space="preserve">23:00</t>
   </si>
   <si>
     <t xml:space="preserve">B6038 - Economía y Organización Industrial</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">8</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">12</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
+    <t xml:space="preserve">8:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00</t>
   </si>
   <si>
     <t xml:space="preserve">B6017 - Seguridad Ambiental</t>
@@ -466,23 +341,7 @@
     <t xml:space="preserve">B6016 - Laboratorio de Sistemas Embebidos</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">18</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
+    <t xml:space="preserve">18:00</t>
   </si>
   <si>
     <t xml:space="preserve">computadoras</t>
@@ -494,23 +353,7 @@
     <t xml:space="preserve">B6000 - Matematica I- Práctica C3</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">:00</t>
-    </r>
+    <t xml:space="preserve">9:00</t>
   </si>
   <si>
     <t xml:space="preserve">B6011 - Física General II</t>
@@ -600,7 +443,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -611,6 +454,18 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -626,15 +481,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -1249,18 +1095,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.25"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1274,59 +1120,347 @@
         <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="C4" s="4"/>
+      <c r="D4" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" s="1" t="n">
+      <c r="D21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>53</v>
+      <c r="E21" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1345,22 +1479,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="51.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="20.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1368,554 +1502,534 @@
         <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="J1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>62</v>
+      <c r="C2" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="F2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>63</v>
+        <v>79</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>69</v>
+      <c r="C5" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>63</v>
+      <c r="C7" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>66</v>
+      <c r="C9" s="6" t="s">
+        <v>83</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>63</v>
+      <c r="C11" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="0" t="s">
+      <c r="H20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Agregado de ejemplo para insertar data y crear views
</commit_message>
<xml_diff>
--- a/src/assets/edificios_default/Universidad.xlsx
+++ b/src/assets/edificios_default/Universidad.xlsx
@@ -367,7 +367,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -394,11 +394,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -443,7 +438,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -461,10 +456,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1479,7 +1470,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
@@ -1513,7 +1504,7 @@
       <c r="E1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>75</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1525,7 +1516,6 @@
       <c r="I1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -1534,7 +1524,7 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1563,7 +1553,7 @@
       <c r="C3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>80</v>
       </c>
       <c r="E3" s="1" t="n">
@@ -1606,7 +1596,7 @@
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>86</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1655,7 +1645,7 @@
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -1704,7 +1694,7 @@
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -1753,7 +1743,7 @@
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D11" s="1" t="s">

</xml_diff>